<commit_message>
Run the Get API
</commit_message>
<xml_diff>
--- a/Resources/TestCaseFiles/WorkFlow.xlsx
+++ b/Resources/TestCaseFiles/WorkFlow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragha\Downloads\Projects\RobotFramework\Resources\TestCaseFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B91F5E4-D063-4E55-B758-2A5CAF3148EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B709BD-DA15-410E-AE52-F3AE3B649617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F7D69B8B-31A6-447D-81E2-6F5B7727590C}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7270" xr2:uid="{F7D69B8B-31A6-447D-81E2-6F5B7727590C}"/>
   </bookViews>
   <sheets>
     <sheet name="Workflow" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>ActionType</t>
   </si>
@@ -80,19 +80,25 @@
 /api/users/2</t>
   </si>
   <si>
-    <t>FirstName=data.first_name</t>
-  </si>
-  <si>
     <t>ActionName</t>
   </si>
   <si>
-    <t>GetFirstName</t>
-  </si>
-  <si>
     <t>GetLastName</t>
   </si>
   <si>
-    <t>LastName=data.last_name</t>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>dummy</t>
+  </si>
+  <si>
+    <t>Name=data[0].employee_name</t>
+  </si>
+  <si>
+    <t>GetEmployeeName</t>
+  </si>
+  <si>
+    <t>/api/users?page=2</t>
   </si>
 </sst>
 </file>
@@ -128,10 +134,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -450,92 +460,96 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.54296875" customWidth="1"/>
     <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.36328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1">
+      <c r="E2" s="2">
         <v>200</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1">
+      <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2">
         <v>200</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1" t="s">
+      <c r="F3" s="2"/>
+      <c r="G3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -545,9 +559,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{105D4BB4-7E5C-4C6C-8E90-1F31D3445162}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -575,6 +591,23 @@
         <v>11</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
code to eject the variable
</commit_message>
<xml_diff>
--- a/Resources/TestCaseFiles/WorkFlow.xlsx
+++ b/Resources/TestCaseFiles/WorkFlow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragha\Downloads\Projects\RobotFramework\Resources\TestCaseFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B709BD-DA15-410E-AE52-F3AE3B649617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB14049-9FCF-4A30-B0E2-C534327A3015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7270" xr2:uid="{F7D69B8B-31A6-447D-81E2-6F5B7727590C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F7D69B8B-31A6-447D-81E2-6F5B7727590C}"/>
   </bookViews>
   <sheets>
     <sheet name="Workflow" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>ActionType</t>
   </si>
@@ -92,13 +92,13 @@
     <t>dummy</t>
   </si>
   <si>
-    <t>Name=data[0].employee_name</t>
-  </si>
-  <si>
     <t>GetEmployeeName</t>
   </si>
   <si>
     <t>/api/users?page=2</t>
+  </si>
+  <si>
+    <t>FirstName=data[0].first_name,LastName=data[0].last_name</t>
   </si>
 </sst>
 </file>
@@ -460,7 +460,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -471,7 +471,7 @@
     <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.36328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.6328125" bestFit="1" customWidth="1"/>
   </cols>
@@ -507,13 +507,13 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>16</v>
@@ -523,7 +523,7 @@
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -545,9 +545,7 @@
         <v>200</v>
       </c>
       <c r="F3" s="2"/>
-      <c r="G3" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>

</xml_diff>